<commit_message>
update terminal run size estimates
</commit_message>
<xml_diff>
--- a/data/run_size/run_size_by_stock_v2.xlsx
+++ b/data/run_size/run_size_by_stock_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\chinAvailability\data\run_size\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836C0D1B-4286-4AB7-A49B-C1AB9FE9B868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394181BD-D0EB-47A9-B1A3-9C8D1855C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6630" windowWidth="29040" windowHeight="15840" xr2:uid="{C0CE7D22-BC85-4388-B131-15B9FE42EBF1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0CE7D22-BC85-4388-B131-15B9FE42EBF1}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_data" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>Luedke, Wilf</author>
   </authors>
   <commentList>
-    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{3AF8F041-1276-473B-A05C-136B77DE3DF8}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{BAF91B7D-4993-4ADB-B660-DC4D2188ABD5}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{41E4D22E-7D95-4FEE-AD61-4AF6A42A33AB}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{E631254A-9F0E-4E33-B5ED-AD287D67AD5E}">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE3" authorId="0" shapeId="0" xr:uid="{8CA5ECD2-82B3-4D2D-A0DE-FB7B58F3CE8C}">
+    <comment ref="AE3" authorId="0" shapeId="0" xr:uid="{B03D0656-565D-4B3D-9CEB-9E75A4729BD8}">
       <text>
         <r>
           <rPr>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG14" authorId="1" shapeId="0" xr:uid="{98A8DA0F-7485-40D5-8EE5-519BB261DC59}">
+    <comment ref="AG14" authorId="1" shapeId="0" xr:uid="{07ED237E-2A6E-4158-A51D-5C8A63061A90}">
       <text>
         <r>
           <rPr>
@@ -473,7 +473,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +541,11 @@
       <sz val="10"/>
       <name val="MS Sans Serif"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="MS Sans Serif"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -588,7 +593,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,6 +617,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -930,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECB6155-C2DE-4A84-8AB9-4208A9CAFBDE}">
   <dimension ref="A1:AM56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:AF56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6239,6 +6247,9 @@
       <c r="Q52">
         <v>328</v>
       </c>
+      <c r="R52" s="15">
+        <v>16609.75</v>
+      </c>
       <c r="S52">
         <v>4319.9078278307597</v>
       </c>
@@ -6349,6 +6360,9 @@
       <c r="Q53">
         <v>371</v>
       </c>
+      <c r="R53" s="15">
+        <v>16609.75</v>
+      </c>
       <c r="S53">
         <v>7121</v>
       </c>
@@ -6459,6 +6473,9 @@
       <c r="Q54">
         <v>285</v>
       </c>
+      <c r="R54" s="15">
+        <v>16609.75</v>
+      </c>
       <c r="S54">
         <v>5080</v>
       </c>
@@ -6569,6 +6586,9 @@
       <c r="Q55">
         <v>439</v>
       </c>
+      <c r="R55" s="15">
+        <v>16609.75</v>
+      </c>
       <c r="S55">
         <v>5487</v>
       </c>
@@ -6634,10 +6654,10 @@
       <c r="A56" s="6">
         <v>2023</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="5">
         <v>14082</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="8">
         <v>29550</v>
       </c>
       <c r="E56" s="10">
@@ -6664,22 +6684,66 @@
       <c r="L56" s="10">
         <v>378000</v>
       </c>
-      <c r="M56">
+      <c r="M56" s="10">
         <v>18136</v>
+      </c>
+      <c r="N56" s="16">
+        <v>29886.25</v>
+      </c>
+      <c r="O56" s="16">
+        <v>1933.75</v>
       </c>
       <c r="P56">
         <v>7481</v>
       </c>
+      <c r="Q56" s="16">
+        <v>355.75</v>
+      </c>
+      <c r="R56" s="15">
+        <v>16609.75</v>
+      </c>
+      <c r="S56" s="16">
+        <v>5501.9769569576902</v>
+      </c>
+      <c r="T56" s="16">
+        <v>1030</v>
+      </c>
+      <c r="U56" s="16">
+        <v>3199.25</v>
+      </c>
       <c r="V56">
         <v>3894</v>
       </c>
       <c r="W56">
         <v>8062</v>
       </c>
+      <c r="X56" s="16">
+        <v>1425.8907104247446</v>
+      </c>
+      <c r="Y56" s="16">
+        <v>7196.2349462137208</v>
+      </c>
+      <c r="Z56" s="17">
+        <v>500</v>
+      </c>
+      <c r="AA56" s="16">
+        <v>54115.671982249551</v>
+      </c>
+      <c r="AB56" s="16">
+        <v>24965.392072971779</v>
+      </c>
+      <c r="AC56" s="16">
+        <v>13494.157942492719</v>
+      </c>
       <c r="AD56">
         <v>16922</v>
       </c>
-      <c r="AF56" s="14"/>
+      <c r="AE56" s="16">
+        <v>14430.701698472687</v>
+      </c>
+      <c r="AF56" s="16">
+        <v>90789.440553358349</v>
+      </c>
       <c r="AG56" s="14">
         <v>342341.5957920074</v>
       </c>

</xml_diff>